<commit_message>
feat(richdocuments): bump to v8.5.12
</commit_message>
<xml_diff>
--- a/apps/richdocuments/emptyTemplates/template.xlsx
+++ b/apps/richdocuments/emptyTemplates/template.xlsx
@@ -24,7 +24,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -44,12 +44,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Source Sans Pro"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -94,12 +88,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -116,7 +106,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -127,14 +117,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-    </row>
-  </sheetData>
+  <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
feat(onlyoffice): use Source Sans Pro font
This reverts commit 67303691089e56fbeafb7eb86ad5966c0547cd5f.
</commit_message>
<xml_diff>
--- a/apps/richdocuments/emptyTemplates/template.xlsx
+++ b/apps/richdocuments/emptyTemplates/template.xlsx
@@ -24,7 +24,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -44,6 +44,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Source Sans Pro"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -88,8 +94,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -106,7 +116,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -117,10 +127,14 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>